<commit_message>
Added snake_case and kebab-case (note UK spelling)
</commit_message>
<xml_diff>
--- a/Denis Robot.xlsx
+++ b/Denis Robot.xlsx
@@ -5,16 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blu3couk-my.sharepoint.com/personal/denis_roberts_blu-3_co_uk/OneDrive/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blu3couk-my.sharepoint.com/personal/denis_roberts_blu-3_co_uk/OneDrive/Training and Reference/Textbooks/OA Robot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="481" documentId="8_{30A52B8C-868B-49E7-87D0-729D8AE88A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{137539B4-6D7A-44AC-BBCB-6008AB77E1D0}"/>
+  <xr:revisionPtr revIDLastSave="791" documentId="8_{30A52B8C-868B-49E7-87D0-729D8AE88A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA92F4CD-EFFE-4352-BC06-4B937F959162}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{23D6A8CF-57FE-4A34-BA04-D39890A7F850}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{23D6A8CF-57FE-4A34-BA04-D39890A7F850}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="5" r:id="rId1"/>
     <sheet name="Ordinals-EN" sheetId="4" r:id="rId2"/>
+    <sheet name="Utilities" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
@@ -49,6 +50,7 @@
     <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
     <definedName name="IQ_TODAY" hidden="1">0</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
+    <definedName name="KebabCase">_xlfn.LAMBDA(_xlpm.input, _xlfn.LET(    _xlpm.\\LambdaName, "KebabCase",    _xlpm.\\CommandName, "Convert To Kebab Case",    _xlpm.\\Description, "Convert text in selection to kebab case.",    _xlpm._Words, Words(_xlpm.input, 1),    _xlpm._Result, _xlfn.TEXTJOIN("-", , LOWER(_xlpm._Words)),    _xlpm._Result ))</definedName>
     <definedName name="OrdinalDate" comment="Convert any date or range of date values into a date in long format, including &quot;th&quot; suffixes.  ">_xlfn.LAMBDA(_xlpm.dates, _xlfn.LET(
    _xlpm.\\LambdaName, "OrdinalDate",
    _xlpm.\\CommandName, "Ordinal Date",
@@ -95,6 +97,13 @@
 ")))), 1),
    _xlpm.r
 ))</definedName>
+    <definedName name="SnakeCase">_xlfn.LAMBDA(_xlpm.input, _xlfn.LET(
+   _xlpm.\\LambdaName, "SnakeCase",
+   _xlpm._Words, Words(_xlpm.input, 1),
+   _xlpm._Result, _xlfn.TEXTJOIN("_", , LOWER(_xlpm._Words)),
+   _xlpm._Result
+))</definedName>
+    <definedName name="Words">_xlfn.LAMBDA(_xlpm.text,_xlop.spill_down, _xlfn.LET(    _xlpm.\\LambdaName, "Words",    _xlpm._Words, _xlfn.TEXTSPLIT(_xlpm.text, " "),    _xlpm._Transpose, IF(_xlfn.ISOMITTED(_xlpm.spill_down), FALSE, _xlpm.spill_down),    _xlpm._Result, IF(_xlpm._Transpose, TRANSPOSE(_xlpm._Words), _xlpm._Words),    _xlpm._Result ))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -139,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="52">
   <si>
     <t>Number</t>
   </si>
@@ -180,12 +189,6 @@
     <t>Denis Robot</t>
   </si>
   <si>
-    <t>Requires selected cells to contain numbers</t>
-  </si>
-  <si>
-    <t>Requires selected cells to contain dates</t>
-  </si>
-  <si>
     <t>Lambda Formula</t>
   </si>
   <si>
@@ -226,6 +229,81 @@
   </si>
   <si>
     <t>How to write a Macro to modify and superscript numbers - Microsoft Community</t>
+  </si>
+  <si>
+    <t>Snake Case</t>
+  </si>
+  <si>
+    <t>Display text in snake case: all lower case, with spaces replaced with underscores</t>
+  </si>
+  <si>
+    <t>Kebab Case</t>
+  </si>
+  <si>
+    <t>Display text in kabob case: all lower case, with spaces replaced with hyphens (this is a rename of kabob case, from the Text Robot command collection)</t>
+  </si>
+  <si>
+    <t>Normal text here</t>
+  </si>
+  <si>
+    <t>NORMAL TEXT HERE</t>
+  </si>
+  <si>
+    <t>normal text here</t>
+  </si>
+  <si>
+    <t>Normal Text Here</t>
+  </si>
+  <si>
+    <t>UPPERCASE</t>
+  </si>
+  <si>
+    <t>Sentence case</t>
+  </si>
+  <si>
+    <t>lower case</t>
+  </si>
+  <si>
+    <t>Proper Case</t>
+  </si>
+  <si>
+    <t>camelCase</t>
+  </si>
+  <si>
+    <t>PascalCase</t>
+  </si>
+  <si>
+    <t>kebab-case</t>
+  </si>
+  <si>
+    <t>snake_case</t>
+  </si>
+  <si>
+    <t>SCREAMING_SNAKE_CASE</t>
+  </si>
+  <si>
+    <t>SCREAMING-KEBAB-CASE</t>
+  </si>
+  <si>
+    <t>normalTextHere</t>
+  </si>
+  <si>
+    <t>NormalTextHere</t>
+  </si>
+  <si>
+    <t>normal-text-here</t>
+  </si>
+  <si>
+    <t>normal_text_here</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>split by words and list by words that works on arrays</t>
+  </si>
+  <si>
+    <t>Naming convention (programming) - Wikipedia</t>
   </si>
 </sst>
 </file>
@@ -378,7 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -419,11 +496,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -431,7 +511,12 @@
     <cellStyle name="Input" xfId="1" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <border>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <bottom/>
@@ -788,10 +873,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD3ECE6-BF56-4000-86E1-CABE04FD5F19}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,137 +884,155 @@
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="120.7109375" customWidth="1"/>
+    <col min="4" max="4" width="135.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="16"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" t="s">
+      <c r="C5" s="18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+      <c r="C7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B22" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>25</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>28</v>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D3">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>OFFSET(A3,0,1)&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:D15">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>OFFSET(B15,0,1)&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:D22">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>OFFSET(B22,0,1)&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -947,22 +1050,22 @@
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="8"/>
-    <col min="3" max="3" width="7.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="7" style="13" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="7"/>
+    <col min="3" max="3" width="7.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="7" style="12" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="7" customWidth="1"/>
     <col min="10" max="10" width="4.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" customWidth="1"/>
     <col min="13" max="13" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.7109375" customWidth="1"/>
@@ -972,161 +1075,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="5" customFormat="1" ht="34.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="6" t="s">
+      <c r="A2" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="4" customFormat="1" ht="34.5" x14ac:dyDescent="0.4">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="6" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="6" t="s">
+      <c r="J5" s="3"/>
+      <c r="K5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4" t="s">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:20" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.4">
-      <c r="B6" s="6"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" s="4" customFormat="1" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="B6" s="5"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" cm="1">
+      <c r="B7" s="6" cm="1">
         <f t="array" ref="B7:B37">_xlfn.SEQUENCE(31)</f>
         <v>1</v>
       </c>
-      <c r="C7" s="13" t="str">
+      <c r="C7" s="12" t="str">
         <f>"st"</f>
         <v>st</v>
       </c>
-      <c r="E7" s="14" cm="1">
+      <c r="E7" s="13" cm="1">
         <f t="array" ref="E7:E37">IF((MOD(_xlfn.ANCHORARRAY(B7), 100) &gt; 10) * (MOD(_xlfn.ANCHORARRAY(B7), 100) &lt; 14), "th", 0)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="14" t="str" cm="1">
+      <c r="F7" s="13" t="str" cm="1">
         <f t="array" ref="F7:F37">_xlfn.SWITCH(MOD(_xlfn.ANCHORARRAY(B7), 10), 1, "st", 2, "nd", 3, "rd", "th")</f>
         <v>st</v>
       </c>
-      <c r="H7" s="8" t="str" cm="1">
+      <c r="H7" s="7" t="str" cm="1">
         <f t="array" ref="H7:H37">OrdinalSuffix(_xlfn.ANCHORARRAY(B7))</f>
         <v>st</v>
       </c>
-      <c r="I7" s="8" t="str" cm="1">
+      <c r="I7" s="7" t="str" cm="1">
         <f t="array" ref="I7:I37">OrdinalNumber(_xlfn.ANCHORARRAY(B7))</f>
         <v>1st</v>
       </c>
-      <c r="K7" s="10" cm="1">
+      <c r="K7" s="9" cm="1">
         <f t="array" ref="K7:K37">DATEVALUE("31/12/2022")+_xlfn.ANCHORARRAY(B7)</f>
         <v>44927</v>
       </c>
-      <c r="M7" s="3" t="str" cm="1">
+      <c r="M7" t="str" cm="1">
         <f t="array" ref="M7:M37">OrdinalDate(_xlfn.ANCHORARRAY(K7))</f>
         <v>Sunday 1st January 2023</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="21" t="str" cm="1">
+      <c r="O7" s="20" t="str" cm="1">
         <f t="array" aca="1" ref="O7" ca="1">ShowFormulas(E7)</f>
         <v>E7: =IF((MOD(B7#, 100) &gt; 10) * (MOD(B7#, 100) &lt; 14), "th", 0)</v>
       </c>
       <c r="T7" s="1"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>2</v>
       </c>
-      <c r="C8" s="13" t="str">
+      <c r="C8" s="12" t="str">
         <f>"nd"</f>
         <v>nd</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>0</v>
       </c>
-      <c r="F8" s="13" t="str">
+      <c r="F8" s="12" t="str">
         <v>nd</v>
       </c>
-      <c r="H8" s="8" t="str">
+      <c r="H8" s="7" t="str">
         <v>nd</v>
       </c>
-      <c r="I8" s="8" t="str">
+      <c r="I8" s="7" t="str">
         <v>2nd</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <v>44928</v>
       </c>
       <c r="M8" t="str">
         <v>Monday 2nd January 2023</v>
       </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="21" t="str" cm="1">
+      <c r="O8" s="20" t="str" cm="1">
         <f t="array" aca="1" ref="O8" ca="1">ShowFormulas(F7)</f>
         <v>F7: =SWITCH(MOD(B7#, 10), 1, "st", 2, "nd", 3, "rd", "th")</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>3</v>
       </c>
-      <c r="C9" s="13" t="str">
+      <c r="C9" s="12" t="str">
         <f>"rd"</f>
         <v>rd</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>0</v>
       </c>
-      <c r="F9" s="13" t="str">
+      <c r="F9" s="12" t="str">
         <v>rd</v>
       </c>
-      <c r="H9" s="8" t="str">
+      <c r="H9" s="7" t="str">
         <v>rd</v>
       </c>
-      <c r="I9" s="8" t="str">
+      <c r="I9" s="7" t="str">
         <v>3rd</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="9">
         <v>44929</v>
       </c>
       <c r="M9" t="str">
@@ -1135,88 +1238,88 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>4</v>
       </c>
-      <c r="C10" s="13" t="str">
+      <c r="C10" s="12" t="str">
         <f>"th"</f>
         <v>th</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>0</v>
       </c>
-      <c r="F10" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H10" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I10" s="8" t="str">
+      <c r="F10" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H10" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I10" s="7" t="str">
         <v>4th</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="9">
         <v>44930</v>
       </c>
       <c r="M10" t="str">
         <v>Wednesday 4th January 2023</v>
       </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="21" t="str" cm="1">
+      <c r="O10" s="20" t="str" cm="1">
         <f t="array" aca="1" ref="O10" ca="1">ShowFormulas(H7)</f>
         <v>H7: =OrdinalSuffix(B7#)</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>5</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>0</v>
       </c>
-      <c r="F11" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H11" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I11" s="8" t="str">
+      <c r="F11" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H11" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I11" s="7" t="str">
         <v>5th</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="9">
         <v>44931</v>
       </c>
       <c r="M11" t="str">
         <v>Thursday 5th January 2023</v>
       </c>
       <c r="N11" s="1"/>
-      <c r="O11" s="21" t="str" cm="1">
+      <c r="O11" s="20" t="str" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">ShowFormulas(I7)</f>
         <v>I7: =OrdinalNumber(B7#)</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>6</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <v>0</v>
       </c>
-      <c r="F12" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H12" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I12" s="8" t="str">
+      <c r="F12" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H12" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I12" s="7" t="str">
         <v>6th</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="9">
         <v>44932</v>
       </c>
       <c r="M12" t="str">
@@ -1225,56 +1328,56 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>7</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <v>0</v>
       </c>
-      <c r="F13" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H13" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I13" s="8" t="str">
+      <c r="F13" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H13" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I13" s="7" t="str">
         <v>7th</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <v>44933</v>
       </c>
       <c r="M13" t="str">
         <v>Saturday 7th January 2023</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="21" t="str" cm="1">
+      <c r="O13" s="20" t="str" cm="1">
         <f t="array" aca="1" ref="O13" ca="1">ShowFormulas(M7)</f>
         <v>M7: =OrdinalDate(K7#)</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>8</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>0</v>
       </c>
-      <c r="F14" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H14" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I14" s="8" t="str">
+      <c r="F14" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H14" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I14" s="7" t="str">
         <v>8th</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="9">
         <v>44934</v>
       </c>
       <c r="M14" t="str">
@@ -1283,25 +1386,25 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>9</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <v>0</v>
       </c>
-      <c r="F15" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H15" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I15" s="8" t="str">
+      <c r="F15" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H15" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I15" s="7" t="str">
         <v>9th</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="9">
         <v>44935</v>
       </c>
       <c r="M15" t="str">
@@ -1310,25 +1413,25 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>10</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <v>0</v>
       </c>
-      <c r="F16" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H16" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I16" s="8" t="str">
+      <c r="F16" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H16" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I16" s="7" t="str">
         <v>10th</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="9">
         <v>44936</v>
       </c>
       <c r="M16" t="str">
@@ -1337,25 +1440,25 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>11</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="F17" s="13" t="str">
+      <c r="E17" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="F17" s="12" t="str">
         <v>st</v>
       </c>
-      <c r="H17" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I17" s="8" t="str">
+      <c r="H17" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I17" s="7" t="str">
         <v>11th</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="9">
         <v>44937</v>
       </c>
       <c r="M17" t="str">
@@ -1364,25 +1467,25 @@
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>12</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="F18" s="13" t="str">
+      <c r="E18" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="F18" s="12" t="str">
         <v>nd</v>
       </c>
-      <c r="H18" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I18" s="8" t="str">
+      <c r="H18" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I18" s="7" t="str">
         <v>12th</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="9">
         <v>44938</v>
       </c>
       <c r="M18" t="str">
@@ -1391,25 +1494,25 @@
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>13</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="F19" s="13" t="str">
+      <c r="E19" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="F19" s="12" t="str">
         <v>rd</v>
       </c>
-      <c r="H19" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I19" s="8" t="str">
+      <c r="H19" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I19" s="7" t="str">
         <v>13th</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="9">
         <v>44939</v>
       </c>
       <c r="M19" t="str">
@@ -1418,25 +1521,25 @@
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>14</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <v>0</v>
       </c>
-      <c r="F20" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H20" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I20" s="8" t="str">
+      <c r="F20" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H20" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I20" s="7" t="str">
         <v>14th</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <v>44940</v>
       </c>
       <c r="M20" t="str">
@@ -1445,25 +1548,25 @@
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>15</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>0</v>
       </c>
-      <c r="F21" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H21" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I21" s="8" t="str">
+      <c r="F21" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H21" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I21" s="7" t="str">
         <v>15th</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="9">
         <v>44941</v>
       </c>
       <c r="M21" t="str">
@@ -1472,25 +1575,25 @@
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>16</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="12">
         <v>0</v>
       </c>
-      <c r="F22" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H22" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I22" s="8" t="str">
+      <c r="F22" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H22" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I22" s="7" t="str">
         <v>16th</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="9">
         <v>44942</v>
       </c>
       <c r="M22" t="str">
@@ -1499,25 +1602,25 @@
       <c r="N22" s="1"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>17</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <v>0</v>
       </c>
-      <c r="F23" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H23" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I23" s="8" t="str">
+      <c r="F23" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H23" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I23" s="7" t="str">
         <v>17th</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="9">
         <v>44943</v>
       </c>
       <c r="M23" t="str">
@@ -1526,25 +1629,25 @@
       <c r="N23" s="1"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>18</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="12">
         <v>0</v>
       </c>
-      <c r="F24" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H24" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I24" s="8" t="str">
+      <c r="F24" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H24" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I24" s="7" t="str">
         <v>18th</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="9">
         <v>44944</v>
       </c>
       <c r="M24" t="str">
@@ -1553,25 +1656,25 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>19</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="12">
         <v>0</v>
       </c>
-      <c r="F25" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H25" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I25" s="8" t="str">
+      <c r="F25" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H25" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I25" s="7" t="str">
         <v>19th</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="9">
         <v>44945</v>
       </c>
       <c r="M25" t="str">
@@ -1580,25 +1683,25 @@
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>20</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="12">
         <v>0</v>
       </c>
-      <c r="F26" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H26" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I26" s="8" t="str">
+      <c r="F26" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H26" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I26" s="7" t="str">
         <v>20th</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="9">
         <v>44946</v>
       </c>
       <c r="M26" t="str">
@@ -1607,25 +1710,25 @@
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>21</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="12">
         <v>0</v>
       </c>
-      <c r="F27" s="13" t="str">
+      <c r="F27" s="12" t="str">
         <v>st</v>
       </c>
-      <c r="H27" s="8" t="str">
+      <c r="H27" s="7" t="str">
         <v>st</v>
       </c>
-      <c r="I27" s="8" t="str">
+      <c r="I27" s="7" t="str">
         <v>21st</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K27" s="9">
         <v>44947</v>
       </c>
       <c r="M27" t="str">
@@ -1634,25 +1737,25 @@
       <c r="N27" s="1"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>22</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="12">
         <v>0</v>
       </c>
-      <c r="F28" s="13" t="str">
+      <c r="F28" s="12" t="str">
         <v>nd</v>
       </c>
-      <c r="H28" s="8" t="str">
+      <c r="H28" s="7" t="str">
         <v>nd</v>
       </c>
-      <c r="I28" s="8" t="str">
+      <c r="I28" s="7" t="str">
         <v>22nd</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="9">
         <v>44948</v>
       </c>
       <c r="M28" t="str">
@@ -1661,25 +1764,25 @@
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>23</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="12">
         <v>0</v>
       </c>
-      <c r="F29" s="13" t="str">
+      <c r="F29" s="12" t="str">
         <v>rd</v>
       </c>
-      <c r="H29" s="8" t="str">
+      <c r="H29" s="7" t="str">
         <v>rd</v>
       </c>
-      <c r="I29" s="8" t="str">
+      <c r="I29" s="7" t="str">
         <v>23rd</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="9">
         <v>44949</v>
       </c>
       <c r="M29" t="str">
@@ -1688,25 +1791,25 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>24</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="12">
         <v>0</v>
       </c>
-      <c r="F30" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H30" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I30" s="8" t="str">
+      <c r="F30" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H30" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I30" s="7" t="str">
         <v>24th</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K30" s="9">
         <v>44950</v>
       </c>
       <c r="M30" t="str">
@@ -1715,25 +1818,25 @@
       <c r="N30" s="1"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>25</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="12">
         <v>0</v>
       </c>
-      <c r="F31" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H31" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I31" s="8" t="str">
+      <c r="F31" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H31" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I31" s="7" t="str">
         <v>25th</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31" s="9">
         <v>44951</v>
       </c>
       <c r="M31" t="str">
@@ -1742,25 +1845,25 @@
       <c r="N31" s="1"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <v>26</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="12">
         <v>0</v>
       </c>
-      <c r="F32" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H32" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I32" s="8" t="str">
+      <c r="F32" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H32" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I32" s="7" t="str">
         <v>26th</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K32" s="9">
         <v>44952</v>
       </c>
       <c r="M32" t="str">
@@ -1769,25 +1872,25 @@
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="7">
+      <c r="B33" s="6">
         <v>27</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="12">
         <v>0</v>
       </c>
-      <c r="F33" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H33" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I33" s="8" t="str">
+      <c r="F33" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H33" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I33" s="7" t="str">
         <v>27th</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K33" s="9">
         <v>44953</v>
       </c>
       <c r="M33" t="str">
@@ -1796,25 +1899,25 @@
       <c r="N33" s="1"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <v>28</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="12">
         <v>0</v>
       </c>
-      <c r="F34" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H34" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I34" s="8" t="str">
+      <c r="F34" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H34" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I34" s="7" t="str">
         <v>28th</v>
       </c>
-      <c r="K34" s="10">
+      <c r="K34" s="9">
         <v>44954</v>
       </c>
       <c r="M34" t="str">
@@ -1823,25 +1926,25 @@
       <c r="N34" s="1"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="7">
+      <c r="B35" s="6">
         <v>29</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="12">
         <v>0</v>
       </c>
-      <c r="F35" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H35" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I35" s="8" t="str">
+      <c r="F35" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H35" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I35" s="7" t="str">
         <v>29th</v>
       </c>
-      <c r="K35" s="10">
+      <c r="K35" s="9">
         <v>44955</v>
       </c>
       <c r="M35" t="str">
@@ -1850,25 +1953,25 @@
       <c r="N35" s="1"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="7">
+      <c r="B36" s="6">
         <v>30</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="12">
         <v>0</v>
       </c>
-      <c r="F36" s="13" t="str">
-        <v>th</v>
-      </c>
-      <c r="H36" s="8" t="str">
-        <v>th</v>
-      </c>
-      <c r="I36" s="8" t="str">
+      <c r="F36" s="12" t="str">
+        <v>th</v>
+      </c>
+      <c r="H36" s="7" t="str">
+        <v>th</v>
+      </c>
+      <c r="I36" s="7" t="str">
         <v>30th</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36" s="9">
         <v>44956</v>
       </c>
       <c r="M36" t="str">
@@ -1877,25 +1980,25 @@
       <c r="N36" s="1"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="7">
+      <c r="B37" s="6">
         <v>31</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="12">
         <v>0</v>
       </c>
-      <c r="F37" s="13" t="str">
+      <c r="F37" s="12" t="str">
         <v>st</v>
       </c>
-      <c r="H37" s="8" t="str">
+      <c r="H37" s="7" t="str">
         <v>st</v>
       </c>
-      <c r="I37" s="8" t="str">
+      <c r="I37" s="7" t="str">
         <v>31st</v>
       </c>
-      <c r="K37" s="10">
+      <c r="K37" s="9">
         <v>44957</v>
       </c>
       <c r="M37" t="str">
@@ -1913,10 +2016,638 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3A5B8C-C24B-4DA3-ADC1-F211CBF4BEF6}">
+  <dimension ref="A1:S20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="7" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C3" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="7" t="str" cm="1">
+        <f t="array" ref="N4:N15">UPPER(K4:K15)</f>
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O4" s="7" t="str" cm="1">
+        <f t="array" ref="O4:O15">UPPER(L4:L15)</f>
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q4" t="str" cm="1">
+        <f t="array" ref="Q4:S4">Words(C4)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R4" t="str">
+        <v>text</v>
+      </c>
+      <c r="S4" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O5" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q5" t="str" cm="1">
+        <f t="array" ref="Q5:S5">Words(C5)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R5" t="str">
+        <v>text</v>
+      </c>
+      <c r="S5" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O6" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q6" t="str" cm="1">
+        <f t="array" ref="Q6:S6">Words(C6)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R6" t="str">
+        <v>text</v>
+      </c>
+      <c r="S6" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O7" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q7" t="str" cm="1">
+        <f t="array" ref="Q7:S7">Words(C7)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R7" t="str">
+        <v>text</v>
+      </c>
+      <c r="S7" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O8" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q8" t="str" cm="1">
+        <f t="array" ref="Q8:S8">Words(C8)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R8" t="str">
+        <v>text</v>
+      </c>
+      <c r="S8" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O9" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q9" t="str" cm="1">
+        <f t="array" ref="Q9:S9">Words(C9)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R9" t="str">
+        <v>text</v>
+      </c>
+      <c r="S9" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O10" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q10" t="str" cm="1">
+        <f t="array" ref="Q10:S10">Words(C10)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R10" t="str">
+        <v>text</v>
+      </c>
+      <c r="S10" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O11" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q11" t="str" cm="1">
+        <f t="array" ref="Q11:S11">Words(C11)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R11" t="str">
+        <v>text</v>
+      </c>
+      <c r="S11" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O12" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q12" t="str" cm="1">
+        <f t="array" ref="Q12:S12">Words(C12)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R12" t="str">
+        <v>text</v>
+      </c>
+      <c r="S12" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N13" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O13" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q13" t="str" cm="1">
+        <f t="array" ref="Q13:S13">Words(C13)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R13" t="str">
+        <v>text</v>
+      </c>
+      <c r="S13" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O14" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q14" t="str" cm="1">
+        <f t="array" ref="Q14:S14">Words(C14)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R14" t="str">
+        <v>text</v>
+      </c>
+      <c r="S14" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N15" s="7" t="str">
+        <v>NORMAL-TEXT-HERE</v>
+      </c>
+      <c r="O15" s="7" t="str">
+        <v>NORMAL_TEXT_HERE</v>
+      </c>
+      <c r="Q15" t="str" cm="1">
+        <f t="array" ref="Q15:S15">Words(C15)</f>
+        <v>Normal</v>
+      </c>
+      <c r="R15" t="str">
+        <v>text</v>
+      </c>
+      <c r="S15" t="str">
+        <v>here</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>OFFSET(A2,0,1)&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C20" r:id="rId1" location="Examples_of_multiple-word_identifier_formats" xr:uid="{610CDC3F-424D-448B-ADC8-AB7A26B8D9F6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <JSON><![CDATA[
 {
   "Commands": [
+    {
+      "Name": "Convert To Kebab Case",
+      "Description": "Convert text in selection to kebab case (lower case, separated by hyphens)",
+      "Type": "ExcelFormulaCommand",
+      "UserContextFilter": "ExcelActiveCellValueIsText",
+      "Formula": "=KebabCase([[ActiveCell::Formula]])",
+      "Tags": [
+        "Convert",
+        "kabob",
+        "kebab"
+      ],
+      "FormulaDependencies": [
+        "KebabCase.lambda",
+        "Words.lambda"
+      ]
+    },
+    {
+      "Name": "Convert to Snake Case",
+      "Description": "Convert the text in selection to Snake Case (lower case, separated by underscores)",
+      "Type": "ExcelFormulaCommand",
+      "Formula": "=SnakeCase([[ActiveCell::Formula]])",
+      "FormulaDependencies": [
+        "SnakeCase.lambda",
+        "Words.lambda"
+      ]
+    },
     {
       "Name": "Ordinal Date",
       "Description": "Convert dates into long format including the ordinal suffixes \"th\", \"st\", \"nd\" and \"rd\"",
@@ -1962,6 +2693,20 @@
       "Location": "GetOrdinalSuffix"
     },
     {
+      "Name": "KabobCase.lambda",
+      "Description": "Definition of KabobCase lambda function.",
+      "Type": "ExcelNameText",
+      "ContentType": "ExcelFormula",
+      "Location": "KabobCase"
+    },
+    {
+      "Name": "KebabCase.lambda",
+      "Description": "Definition of KebabCase lambda function.",
+      "Type": "ExcelNameText",
+      "ContentType": "ExcelFormula",
+      "Location": "KebabCase"
+    },
+    {
       "Name": "OrdinalDate.lambda",
       "Description": "Definition of OrdinalDate lambda function.",
       "Type": "ExcelNameText",
@@ -1988,38 +2733,32 @@
       "Type": "ExcelNameText",
       "ContentType": "ExcelFormula",
       "Location": "ShowFormulas"
+    },
+    {
+      "Name": "SnakeCase.lambda",
+      "Description": "Definition of SnakeCase lambda function.",
+      "Type": "ExcelNameText",
+      "ContentType": "ExcelFormula",
+      "Location": "SnakeCase"
+    },
+    {
+      "Name": "Words.lambda",
+      "Description": "Definition of Words lambda function.",
+      "Type": "ExcelNameText",
+      "ContentType": "ExcelFormula",
+      "Location": "Words"
     }
   ]
 }
 ]]></JSON>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item10.xml><?xml version="1.0" encoding="utf-8"?>
 <Text><![CDATA[
 ]]></Text>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<Text><![CDATA[
-]]></Text>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<Text><![CDATA[
-]]></Text>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<Text><![CDATA[
-]]></Text>
-</file>
-
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<Text><![CDATA[
-]]></Text>
-</file>
-
-<file path=customXml/item7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item11.xml><?xml version="1.0" encoding="utf-8"?>
 <writeIndexDataTable>
   <xs:schema xmlns="" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:msdata="urn:schemas-microsoft-com:xml-msdata" id="writeIndexDataTable">
     <xs:element name="writeIndexDataTable" msdata:IsDataSet="true" msdata:UseCurrentLocale="true">
@@ -2052,8 +2791,8 @@
     <ItemName>HotkeyCommands</ItemName>
     <ItemDescription/>
     <ItemType>JSON</ItemType>
-    <LastUpdated>19/06/2025 12:43:52 +01:00</LastUpdated>
-    <CustomXmlPartGuid>{82A4ABE1-8856-43F8-A28F-AC39E0F97CCB}</CustomXmlPartGuid>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{EB259F73-0872-4AE0-91E7-3F98382A8DA8}</CustomXmlPartGuid>
   </CustomXmlPartIndex>
   <CustomXmlPartIndex>
     <CollectionName>HotkeyCommands</CollectionName>
@@ -2061,8 +2800,17 @@
     <ItemDescription/>
     <ItemType>Text</ItemType>
     <ItemSubtype/>
-    <LastUpdated>19/06/2025 12:43:52 +01:00</LastUpdated>
-    <CustomXmlPartGuid>{5DDC3BA1-CD3D-4622-BF15-0EB1BFA9B1B2}</CustomXmlPartGuid>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{C230EA9D-850B-4245-9F0B-75B41EA47DCD}</CustomXmlPartGuid>
+  </CustomXmlPartIndex>
+  <CustomXmlPartIndex>
+    <CollectionName>HotkeyCommands</CollectionName>
+    <ItemName>KebabCase.lambda</ItemName>
+    <ItemDescription/>
+    <ItemType>Text</ItemType>
+    <ItemSubtype/>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{8D6F1B1E-026B-4230-8FEE-F3808BAC19A4}</CustomXmlPartGuid>
   </CustomXmlPartIndex>
   <CustomXmlPartIndex>
     <CollectionName>HotkeyCommands</CollectionName>
@@ -2070,8 +2818,8 @@
     <ItemDescription/>
     <ItemType>Text</ItemType>
     <ItemSubtype/>
-    <LastUpdated>19/06/2025 12:43:52 +01:00</LastUpdated>
-    <CustomXmlPartGuid>{AD4B1954-17ED-4764-BFDE-4B72F98C5FFE}</CustomXmlPartGuid>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{1207116D-20EB-4E06-A736-6D0B046579C8}</CustomXmlPartGuid>
   </CustomXmlPartIndex>
   <CustomXmlPartIndex>
     <CollectionName>HotkeyCommands</CollectionName>
@@ -2079,8 +2827,8 @@
     <ItemDescription/>
     <ItemType>Text</ItemType>
     <ItemSubtype/>
-    <LastUpdated>19/06/2025 12:43:52 +01:00</LastUpdated>
-    <CustomXmlPartGuid>{0183378B-3F2C-4E1D-985B-26F335D3ACF0}</CustomXmlPartGuid>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{45C38149-7830-4853-A705-29BCF9AEFB8D}</CustomXmlPartGuid>
   </CustomXmlPartIndex>
   <CustomXmlPartIndex>
     <CollectionName>HotkeyCommands</CollectionName>
@@ -2088,8 +2836,8 @@
     <ItemDescription/>
     <ItemType>Text</ItemType>
     <ItemSubtype/>
-    <LastUpdated>19/06/2025 12:43:52 +01:00</LastUpdated>
-    <CustomXmlPartGuid>{6C7810E5-AF51-4D93-9261-5A92615966F8}</CustomXmlPartGuid>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{F02AB860-EEAD-43DB-8563-F1FFD74F1E6F}</CustomXmlPartGuid>
   </CustomXmlPartIndex>
   <CustomXmlPartIndex>
     <CollectionName>HotkeyCommands</CollectionName>
@@ -2097,54 +2845,155 @@
     <ItemDescription/>
     <ItemType>Text</ItemType>
     <ItemSubtype/>
-    <LastUpdated>19/06/2025 12:43:52 +01:00</LastUpdated>
-    <CustomXmlPartGuid>{4BC3F9A5-875C-47E9-96A3-7F0478F364DD}</CustomXmlPartGuid>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{0AAA429B-206E-4EAE-B790-AAD07B77E512}</CustomXmlPartGuid>
+  </CustomXmlPartIndex>
+  <CustomXmlPartIndex>
+    <CollectionName>HotkeyCommands</CollectionName>
+    <ItemName>KabobCase.lambda</ItemName>
+    <ItemDescription/>
+    <ItemType>Text</ItemType>
+    <ItemSubtype/>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{0053F7D5-D036-493C-A3C1-440C87D50BFC}</CustomXmlPartGuid>
+  </CustomXmlPartIndex>
+  <CustomXmlPartIndex>
+    <CollectionName>HotkeyCommands</CollectionName>
+    <ItemName>SnakeCase.lambda</ItemName>
+    <ItemDescription/>
+    <ItemType>Text</ItemType>
+    <ItemSubtype/>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{D8A61416-D790-438B-A2DA-2CF1978C8E33}</CustomXmlPartGuid>
+  </CustomXmlPartIndex>
+  <CustomXmlPartIndex>
+    <CollectionName>HotkeyCommands</CollectionName>
+    <ItemName>Words.lambda</ItemName>
+    <ItemDescription/>
+    <ItemType>Text</ItemType>
+    <ItemSubtype/>
+    <LastUpdated>19/06/2025 15:26:23 +01:00</LastUpdated>
+    <CustomXmlPartGuid>{FB2007D8-6EEC-45D5-B8AA-799201839A7C}</CustomXmlPartGuid>
   </CustomXmlPartIndex>
 </writeIndexDataTable>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<Text><![CDATA[
+]]></Text>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<Text><![CDATA[
+KebabCase = LAMBDA(input, LET(    \\LambdaName, "KebabCase",    \\CommandName, "Convert To Kebab Case",    \\Description, "Convert text in selection to kebab case.",    _Words, Words(input, 1),    _Result, TEXTJOIN("-", , LOWER(_Words)),    _Result ));
+]]></Text>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<Text><![CDATA[
+]]></Text>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<Text><![CDATA[
+]]></Text>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<Text><![CDATA[
+]]></Text>
+</file>
+
+<file path=customXml/item7.xml><?xml version="1.0" encoding="utf-8"?>
+<Text><![CDATA[
+]]></Text>
+</file>
+
+<file path=customXml/item8.xml><?xml version="1.0" encoding="utf-8"?>
+<Text><![CDATA[
+/*Convert text in selection to kabob case.  */
+KabobCase = LAMBDA(input, LET(
+   \\LambdaName, "KabobCase",
+   \\CommandName, "Convert To Kabob Case",
+   \\Description, "Convert text in selection to kabob case.",
+   _Words, Words(input, 1),
+   _Result, TEXTJOIN("-", , LOWER(_Words)),
+   _Result
+));
+]]></Text>
+</file>
+
+<file path=customXml/item9.xml><?xml version="1.0" encoding="utf-8"?>
+<Text><![CDATA[
+]]></Text>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82A4ABE1-8856-43F8-A28F-AC39E0F97CCB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB259F73-0872-4AE0-91E7-3F98382A8DA8}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DDC3BA1-CD3D-4622-BF15-0EB1BFA9B1B2}">
+<file path=customXml/itemProps10.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2007D8-6EEC-45D5-B8AA-799201839A7C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD4B1954-17ED-4764-BFDE-4B72F98C5FFE}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0183378B-3F2C-4E1D-985B-26F335D3ACF0}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C7810E5-AF51-4D93-9261-5A92615966F8}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BC3F9A5-875C-47E9-96A3-7F0478F364DD}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps7.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1204F272-A591-4DB1-B3FD-EEAE2537F3C7}">
+<file path=customXml/itemProps11.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90AC157C-EA33-48C5-8B80-AE693A57DED9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri=""/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="urn:schemas-microsoft-com:xml-msdata"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C230EA9D-850B-4245-9F0B-75B41EA47DCD}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D6F1B1E-026B-4230-8FEE-F3808BAC19A4}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1207116D-20EB-4E06-A736-6D0B046579C8}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45C38149-7830-4853-A705-29BCF9AEFB8D}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02AB860-EEAD-43DB-8563-F1FFD74F1E6F}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps7.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AAA429B-206E-4EAE-B790-AAD07B77E512}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps8.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0053F7D5-D036-493C-A3C1-440C87D50BFC}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps9.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A61416-D790-438B-A2DA-2CF1978C8E33}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
</xml_diff>